<commit_message>
update no scopes excel
</commit_message>
<xml_diff>
--- a/scopes.xlsx
+++ b/scopes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Code\ainetproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ainetproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>comment</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>scopeActive</t>
+  </si>
+  <si>
+    <t>substituir com o laravel scout</t>
+  </si>
+  <si>
+    <t>printers</t>
   </si>
 </sst>
 </file>
@@ -448,15 +454,17 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="65.25" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,6 +476,9 @@
       </c>
       <c r="E1" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -499,15 +510,21 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>

</xml_diff>